<commit_message>
Custom Report Feature Updated through IReporter
</commit_message>
<xml_diff>
--- a/SpreadSheetReports/ResultSummary.xlsx
+++ b/SpreadSheetReports/ResultSummary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -32,7 +32,7 @@
     <t>testCase1</t>
   </si>
   <si>
-    <t>04-Jan-2020 04:48:19</t>
+    <t>05-Jan-2020 02:07:31</t>
   </si>
   <si>
     <t>Pass</t>
@@ -47,10 +47,7 @@
     <t>test01</t>
   </si>
   <si>
-    <t>04-Jan-2020 04:48:25</t>
-  </si>
-  <si>
-    <t>04-Jan-2020 04:48:26</t>
+    <t>05-Jan-2020 02:07:40</t>
   </si>
 </sst>
 </file>
@@ -215,7 +212,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s" s="3">
         <v>7</v>

</xml_diff>